<commit_message>
Almost Finished Manual Interaction Mode
-Just need to add the boolean modification to the button presses.
-Added request handler to Arduino Mega.
-Added motor control functions to Arduino Mega
-Added serial communication to Arduino Mega
</commit_message>
<xml_diff>
--- a/Documentation/Request_List.xlsx
+++ b/Documentation/Request_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34FE589-FD81-4B9C-B521-A3204F2E6DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E4B0E-3817-4CDB-9D87-F5FB1B3B77A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,6 +489,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,21 +520,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,7 +805,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,34 +825,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
       <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,27 +873,27 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="26"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="31"/>
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1125,32 +1125,32 @@
       <c r="F7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29" t="s">
+      <c r="K7" s="22"/>
+      <c r="L7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="31"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="25"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1373,6 +1373,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:X1"/>
+    <mergeCell ref="F2:X2"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:X7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:X5"/>
+    <mergeCell ref="G6:X6"/>
     <mergeCell ref="K11:X11"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="H10:X10"/>
@@ -1380,19 +1393,6 @@
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:X9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:X7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:X5"/>
-    <mergeCell ref="G6:X6"/>
-    <mergeCell ref="G4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:X1"/>
-    <mergeCell ref="F2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started adding interaction mode functionality
-Added autonomous extraction of data and sending it to the controller client.
</commit_message>
<xml_diff>
--- a/Documentation/Request_List.xlsx
+++ b/Documentation/Request_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E4B0E-3817-4CDB-9D87-F5FB1B3B77A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09444797-93E0-47C3-991E-0ACE8ADF0E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Request ID</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>The Sender ID does not need to be sent from the client controller as the server knows which controller client has sent the request.</t>
+  </si>
+  <si>
+    <t>InteractionMode</t>
+  </si>
+  <si>
+    <t>Changes the interaction mode between the controller client and the buggy.</t>
+  </si>
+  <si>
+    <t>Buggy (Arduino/ESP32)</t>
+  </si>
+  <si>
+    <t>Interaction Mode</t>
   </si>
 </sst>
 </file>
@@ -439,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,7 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,6 +500,24 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,23 +533,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,7 +828,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +839,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
@@ -825,34 +848,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
       <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
@@ -872,28 +895,28 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="31"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="25"/>
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -909,64 +932,64 @@
       <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>2</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>3</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>4</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>5</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>6</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>7</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="11">
         <v>8</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <v>9</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <v>10</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="Q3" s="11">
         <v>11</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="11">
         <v>12</v>
       </c>
-      <c r="S3" s="12">
+      <c r="S3" s="11">
         <v>13</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="11">
         <v>14</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <v>15</v>
       </c>
-      <c r="V3" s="12">
+      <c r="V3" s="11">
         <v>16</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="11">
         <v>17</v>
       </c>
-      <c r="X3" s="12">
+      <c r="X3" s="11">
         <v>18</v>
       </c>
       <c r="Y3" s="4"/>
@@ -981,41 +1004,41 @@
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="18" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="18" t="s">
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="18" t="s">
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="20"/>
+      <c r="X4" s="19"/>
       <c r="Y4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1030,37 +1053,37 @@
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="18" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="20"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="19"/>
       <c r="Y5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1075,35 +1098,35 @@
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="20"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="19"/>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1116,41 +1139,41 @@
       <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="15" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23" t="s">
+      <c r="K7" s="27"/>
+      <c r="L7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="25"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="30"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1163,37 +1186,37 @@
       <c r="C8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="20"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="19"/>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1206,39 +1229,39 @@
       <c r="C9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="18" t="s">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="18" t="s">
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="20"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="19"/>
       <c r="Y9" s="3" t="s">
         <v>43</v>
       </c>
@@ -1253,37 +1276,37 @@
       <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="20"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="19"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1296,40 +1319,80 @@
       <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="18" t="s">
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="20"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="19"/>
       <c r="Y11" s="3"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="9">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="19"/>
       <c r="Y12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -1372,7 +1435,21 @@
       <c r="Y25" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="H12:X12"/>
+    <mergeCell ref="K11:X11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="H10:X10"/>
+    <mergeCell ref="H8:X8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:X9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:X7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:X5"/>
+    <mergeCell ref="G6:X6"/>
     <mergeCell ref="G4:N4"/>
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="S4:V4"/>
@@ -1380,19 +1457,6 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:X1"/>
     <mergeCell ref="F2:X2"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:X7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:X5"/>
-    <mergeCell ref="G6:X6"/>
-    <mergeCell ref="K11:X11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="H10:X10"/>
-    <mergeCell ref="H8:X8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:X9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chnaged arduino Request handler
</commit_message>
<xml_diff>
--- a/Documentation/Request_List.xlsx
+++ b/Documentation/Request_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09444797-93E0-47C3-991E-0ACE8ADF0E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19599866-1559-4562-BB79-59E6A886E10F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>Request ID</t>
   </si>
@@ -169,6 +169,42 @@
   </si>
   <si>
     <t>Interaction Mode</t>
+  </si>
+  <si>
+    <t>CurrConfigParam</t>
+  </si>
+  <si>
+    <t>requests the current configuration parameter for the selcted configuration options in configuration interaction mode.</t>
+  </si>
+  <si>
+    <t>Configuration Option</t>
+  </si>
+  <si>
+    <t>SendCurrConfig</t>
+  </si>
+  <si>
+    <t>Sends the current configuration of the option.</t>
+  </si>
+  <si>
+    <t>Current Conifguration Parameter</t>
+  </si>
+  <si>
+    <t>UpdateConfigOption</t>
+  </si>
+  <si>
+    <t>Updates the selected configuration option with the selected configuration parameter.</t>
+  </si>
+  <si>
+    <t>Configuration Parameter</t>
+  </si>
+  <si>
+    <t>ConfigUpdateStatus</t>
+  </si>
+  <si>
+    <t>Sends the result of the update of the configuration option.</t>
+  </si>
+  <si>
+    <t>Update Status</t>
   </si>
 </sst>
 </file>
@@ -208,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,8 +281,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -447,11 +489,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,6 +556,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,6 +576,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,32 +600,59 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +937,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,34 +957,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
       <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
@@ -896,27 +1005,27 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="25"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="31"/>
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -995,7 +1104,7 @@
       <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -1004,47 +1113,47 @@
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="17" t="s">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="17" t="s">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="17" t="s">
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="19"/>
+      <c r="X4" s="23"/>
       <c r="Y4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="9">
@@ -1053,43 +1162,43 @@
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="17" t="s">
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="19"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="35"/>
       <c r="Y5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="44" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="9">
@@ -1098,39 +1207,39 @@
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="19"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="35"/>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="9">
@@ -1139,45 +1248,45 @@
       <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="28" t="s">
+      <c r="K7" s="25"/>
+      <c r="L7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="30"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
+      <c r="X7" s="38"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="44" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="9">
@@ -1186,10 +1295,10 @@
       <c r="C8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -1198,29 +1307,29 @@
       <c r="G8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="19"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="35"/>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="9">
@@ -1229,45 +1338,45 @@
       <c r="C9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="19" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="17" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="17" t="s">
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="19"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="35"/>
       <c r="Y9" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="44" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="9">
@@ -1276,10 +1385,10 @@
       <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="15" t="s">
@@ -1288,29 +1397,29 @@
       <c r="G10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="19"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="35"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="44" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="9">
@@ -1319,41 +1428,41 @@
       <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="17" t="s">
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="19"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="35"/>
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="44" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="9">
@@ -1362,80 +1471,262 @@
       <c r="C12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="19" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="19"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="35"/>
       <c r="Y12" s="3"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="9">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="35"/>
       <c r="Y13" s="3"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="32">
+        <v>11</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="35"/>
       <c r="Y14" s="3"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="9">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="35"/>
       <c r="Y15" s="3"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="9">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="35"/>
       <c r="Y16" s="3"/>
     </row>
-    <row r="17" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y17" s="3"/>
     </row>
-    <row r="18" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y19" s="3"/>
     </row>
-    <row r="20" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y20" s="3"/>
     </row>
-    <row r="21" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y21" s="3"/>
     </row>
-    <row r="22" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y22" s="3"/>
     </row>
-    <row r="23" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y23" s="3"/>
     </row>
-    <row r="24" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y24" s="3"/>
     </row>
-    <row r="25" spans="25:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
       <c r="Y25" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="27">
+    <mergeCell ref="H16:X16"/>
+    <mergeCell ref="H13:X13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:X14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:X15"/>
+    <mergeCell ref="G4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:X1"/>
+    <mergeCell ref="F2:X2"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:X7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:X5"/>
+    <mergeCell ref="G6:X6"/>
     <mergeCell ref="H12:X12"/>
     <mergeCell ref="K11:X11"/>
     <mergeCell ref="G11:J11"/>
@@ -1444,19 +1735,6 @@
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:X9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:X7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:X5"/>
-    <mergeCell ref="G6:X6"/>
-    <mergeCell ref="G4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:X1"/>
-    <mergeCell ref="F2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commented and tidied some code up
-Commented ESP32 buggy sketch
-Added some functionality to reconnect the buggy automatically to the server upon disconnection
-When buggy disconnects from server or client itt now goes into manual mode automatically to precent it from driving around on its own without any way to stop it.
</commit_message>
<xml_diff>
--- a/Documentation/Request_List.xlsx
+++ b/Documentation/Request_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9017CCBF-1A08-43AD-BEEF-A533B9AAFFC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F97CC9-0422-4DBF-A6E6-245B4A27A223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
   <si>
     <t>Request ID</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>BuggyDisconnect</t>
+  </si>
+  <si>
+    <t>IsAlive</t>
+  </si>
+  <si>
+    <t>Sent to all connected clients periodically to determine whether connection is still active or whether a disconnection has occurred.</t>
+  </si>
+  <si>
+    <t>Controller Client/Buggy</t>
   </si>
 </sst>
 </file>
@@ -616,6 +625,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -623,48 +674,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,7 +958,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,34 +978,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
       <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1017,27 +1026,27 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="46"/>
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1134,32 +1143,32 @@
       <c r="F4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="36" t="s">
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="36" t="s">
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="36" t="s">
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="38"/>
+      <c r="X4" s="35"/>
       <c r="Y4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1183,12 +1192,12 @@
       <c r="F5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35"/>
       <c r="K5" s="30" t="s">
         <v>8</v>
       </c>
@@ -1269,32 +1278,32 @@
       <c r="F7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="37"/>
+      <c r="L7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="49"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="40"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1359,18 +1368,18 @@
       <c r="F9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="36" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="38"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="35"/>
       <c r="O9" s="30" t="s">
         <v>8</v>
       </c>
@@ -1449,12 +1458,12 @@
       <c r="F11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="30" t="s">
         <v>8</v>
       </c>
@@ -1578,12 +1587,12 @@
       <c r="F14" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="49"/>
       <c r="K14" s="30" t="s">
         <v>8</v>
       </c>
@@ -1624,12 +1633,12 @@
       <c r="G15" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="30" t="s">
         <v>8</v>
       </c>
@@ -1774,8 +1783,45 @@
       <c r="X18" s="32"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
+    <row r="19" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="32"/>
       <c r="Y19" s="3"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -1801,7 +1847,29 @@
       <c r="Y25" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="G19:X19"/>
+    <mergeCell ref="H18:X18"/>
+    <mergeCell ref="G17:X17"/>
+    <mergeCell ref="H16:X16"/>
+    <mergeCell ref="H13:X13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:X14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:X15"/>
+    <mergeCell ref="G4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:X1"/>
+    <mergeCell ref="F2:X2"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:X7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:X5"/>
+    <mergeCell ref="G6:X6"/>
     <mergeCell ref="H12:X12"/>
     <mergeCell ref="K11:X11"/>
     <mergeCell ref="G11:J11"/>
@@ -1810,27 +1878,6 @@
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:X9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:X7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:X5"/>
-    <mergeCell ref="G6:X6"/>
-    <mergeCell ref="G4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:X1"/>
-    <mergeCell ref="F2:X2"/>
-    <mergeCell ref="H18:X18"/>
-    <mergeCell ref="G17:X17"/>
-    <mergeCell ref="H16:X16"/>
-    <mergeCell ref="H13:X13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:X14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:X15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tested the System and updated test sheet.
</commit_message>
<xml_diff>
--- a/Documentation/Request_List.xlsx
+++ b/Documentation/Request_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B40510-2FAE-421C-B267-BF61058451B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F90A49D-EAC1-4450-9FC2-627C2746C2EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,14 +618,59 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -635,51 +680,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,8 +966,8 @@
   </sheetPr>
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,34 +987,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -1033,27 +1033,27 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="44"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="47"/>
       <c r="Y2" s="29"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1150,32 +1150,32 @@
       <c r="F4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="36" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="36" t="s">
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="30" t="s">
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="32"/>
+      <c r="X4" s="34"/>
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1197,28 +1197,28 @@
       <c r="F5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="30" t="s">
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="32"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="34"/>
       <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1240,26 +1240,26 @@
       <c r="F6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="32"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="34"/>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1281,32 +1281,32 @@
       <c r="F7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="38"/>
+      <c r="L7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="49"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="41"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1331,25 +1331,25 @@
       <c r="G8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="32"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="34"/>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1371,30 +1371,30 @@
       <c r="F9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="36" t="s">
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="30" t="s">
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="32"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="34"/>
       <c r="Y9" s="3"/>
     </row>
     <row r="10" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1419,25 +1419,25 @@
       <c r="G10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="32"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="34"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1459,28 +1459,28 @@
       <c r="F11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="30" t="s">
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="31"/>
-      <c r="X11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="34"/>
       <c r="Y11" s="3"/>
     </row>
     <row r="12" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1505,25 +1505,25 @@
       <c r="G12" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="34"/>
       <c r="Y12" s="3"/>
     </row>
     <row r="13" spans="1:35" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1548,25 +1548,25 @@
       <c r="G13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="34"/>
       <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1588,28 +1588,28 @@
       <c r="F14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="30" t="s">
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="32"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="34"/>
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1634,27 +1634,27 @@
       <c r="G15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="30" t="s">
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="34"/>
       <c r="Y15" s="3"/>
     </row>
     <row r="16" spans="1:35" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1679,25 +1679,25 @@
       <c r="G16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="34"/>
       <c r="Y16" s="3"/>
     </row>
     <row r="17" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1719,26 +1719,26 @@
       <c r="F17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="34"/>
       <c r="Y17" s="3"/>
     </row>
     <row r="18" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1763,25 +1763,25 @@
       <c r="G18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="34"/>
       <c r="Y18" s="3"/>
     </row>
     <row r="19" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1803,26 +1803,26 @@
       <c r="F19" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="34"/>
       <c r="Y19" s="3"/>
     </row>
     <row r="20" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1832,7 +1832,7 @@
       <c r="B20" s="8">
         <v>16</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="30" t="s">
         <v>66</v>
       </c>
       <c r="D20" s="19" t="s">
@@ -1847,27 +1847,27 @@
       <c r="G20" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="31" t="s">
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="32"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="34"/>
       <c r="Y20" s="3"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -1890,22 +1890,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:X20"/>
-    <mergeCell ref="H12:X12"/>
-    <mergeCell ref="K11:X11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="H10:X10"/>
-    <mergeCell ref="H8:X8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:X9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:X7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:X5"/>
-    <mergeCell ref="G6:X6"/>
     <mergeCell ref="G4:N4"/>
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="S4:V4"/>
@@ -1913,6 +1897,22 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:X1"/>
     <mergeCell ref="F2:X2"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:X7"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:X5"/>
+    <mergeCell ref="G6:X6"/>
+    <mergeCell ref="H10:X10"/>
+    <mergeCell ref="H8:X8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:X9"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:X20"/>
+    <mergeCell ref="H12:X12"/>
+    <mergeCell ref="K11:X11"/>
+    <mergeCell ref="G11:J11"/>
     <mergeCell ref="G19:X19"/>
     <mergeCell ref="H18:X18"/>
     <mergeCell ref="G17:X17"/>

</xml_diff>